<commit_message>
semana 04 - r
</commit_message>
<xml_diff>
--- a/img/aula03/croqui_anova.xlsx
+++ b/img/aula03/croqui_anova.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -434,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:A25"/>
     </sheetView>
   </sheetViews>

</xml_diff>